<commit_message>
toevoegen overstromings check, schade kosten
</commit_message>
<xml_diff>
--- a/data/houses.xlsx
+++ b/data/houses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/gvandiggelen_tudelft_nl/Documents/BEP_WWM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{F86210D8-2D5E-45A0-B339-F4CBD9C9C1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9DC6A75-C82D-4CAA-9293-076ADC054A22}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{F86210D8-2D5E-45A0-B339-F4CBD9C9C1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3B807AC-4A9D-4CF9-A51A-8C2A795F660D}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="9307" xr2:uid="{BDD7B449-AB1F-456A-93BA-B17D2D0F1B48}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{BDD7B449-AB1F-456A-93BA-B17D2D0F1B48}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>house_id</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>rain_protection</t>
+  </si>
+  <si>
+    <t>river_protection</t>
   </si>
 </sst>
 </file>
@@ -109,6 +115,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,15 +438,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EDA5C8-35D3-4400-87E5-E5E127CEDEB2}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.9296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,16 +460,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -461,16 +483,22 @@
         <v>300000</v>
       </c>
       <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -478,12 +506,18 @@
         <v>300000</v>
       </c>
       <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
toevoegen huizen, agenten en visualisatie in model.py
</commit_message>
<xml_diff>
--- a/data/houses.xlsx
+++ b/data/houses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/gvandiggelen_tudelft_nl/Documents/BEP_WWM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{F86210D8-2D5E-45A0-B339-F4CBD9C9C1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3B807AC-4A9D-4CF9-A51A-8C2A795F660D}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="8_{F86210D8-2D5E-45A0-B339-F4CBD9C9C1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6D6289F-CBA2-48FF-A8AD-B82AA83106E4}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{BDD7B449-AB1F-456A-93BA-B17D2D0F1B48}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>house_id</t>
   </si>
@@ -63,6 +63,108 @@
   </si>
   <si>
     <t>river_protection</t>
+  </si>
+  <si>
+    <t>N01</t>
+  </si>
+  <si>
+    <t>N04</t>
+  </si>
+  <si>
+    <t>N05</t>
+  </si>
+  <si>
+    <t>N07</t>
+  </si>
+  <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>D02</t>
+  </si>
+  <si>
+    <t>D04</t>
+  </si>
+  <si>
+    <t>D05</t>
+  </si>
+  <si>
+    <t>D09</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>U01</t>
+  </si>
+  <si>
+    <t>U04</t>
+  </si>
+  <si>
+    <t>U05</t>
+  </si>
+  <si>
+    <t>U09</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>N02</t>
+  </si>
+  <si>
+    <t>N03</t>
+  </si>
+  <si>
+    <t>N06</t>
+  </si>
+  <si>
+    <t>D03</t>
+  </si>
+  <si>
+    <t>D06</t>
+  </si>
+  <si>
+    <t>D07</t>
+  </si>
+  <si>
+    <t>D08</t>
+  </si>
+  <si>
+    <t>U02</t>
+  </si>
+  <si>
+    <t>U03</t>
+  </si>
+  <si>
+    <t>U06</t>
+  </si>
+  <si>
+    <t>U07</t>
+  </si>
+  <si>
+    <t>U08</t>
+  </si>
+  <si>
+    <t>[Self-activating wall]</t>
+  </si>
+  <si>
+    <t>[Self-activating wall, Rain barrel]</t>
+  </si>
+  <si>
+    <t>[Sandbags]</t>
+  </si>
+  <si>
+    <t>[Waterproofing walls &amp; floors, Self-activating wall]</t>
+  </si>
+  <si>
+    <t>[Green garden, Waterproofing walls &amp; floors]</t>
+  </si>
+  <si>
+    <t>[Self-activating wall, Waterproofing walls &amp; floors]</t>
+  </si>
+  <si>
+    <t>available_round</t>
   </si>
 </sst>
 </file>
@@ -438,86 +540,746 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EDA5C8-35D3-4400-87E5-E5E127CEDEB2}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>425000</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>200000</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>200000</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>100000</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>300000</v>
       </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2">
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>300000</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>160000</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>160000</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>80000</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>80000</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>200000</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>125000</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>125000</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>70000</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>70000</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>200000</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>425000</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>100000</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
         <v>300000</v>
       </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
+      <c r="D20">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>160000</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>160000</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>80000</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>200000</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>200000</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>125000</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>125000</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>41</v>
+      </c>
+      <c r="H27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>70000</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
toevoegen policys, nieuwe grafieken en verwijderen policy bestand
</commit_message>
<xml_diff>
--- a/data/houses.xlsx
+++ b/data/houses.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="174" documentId="8_{F86210D8-2D5E-45A0-B339-F4CBD9C9C1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6D6289F-CBA2-48FF-A8AD-B82AA83106E4}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{BDD7B449-AB1F-456A-93BA-B17D2D0F1B48}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="16200" windowHeight="9307" xr2:uid="{BDD7B449-AB1F-456A-93BA-B17D2D0F1B48}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -217,6 +217,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -539,7 +543,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H28"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>